<commit_message>
changed line 66-69 app.py
</commit_message>
<xml_diff>
--- a/RESMED_DATABASE_060525.xlsx
+++ b/RESMED_DATABASE_060525.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TAS Xavier\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TAS Xavier\Desktop\QR Custom\easmed_qr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E264A340-D88A-4802-9EB2-19908B8B3C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46520060-2656-4600-A014-A75F68E87496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7718D232-6125-43CE-AFDE-9C4FAF0200A9}"/>
   </bookViews>
@@ -2211,19 +2211,19 @@
     <t>619498000104</t>
   </si>
   <si>
-    <t>RESMED SKU</t>
-  </si>
-  <si>
-    <t>RESMED DESCRIPTION</t>
-  </si>
-  <si>
     <t>ITEM TRACKING CODE</t>
   </si>
   <si>
-    <t>RESMED GTIN</t>
-  </si>
-  <si>
     <t>010061949863859811231213101753445</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SKU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DESCRIPTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GTIN</t>
   </si>
 </sst>
 </file>
@@ -2445,8 +2445,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6C54116F-5E15-4235-9D70-EC1EDF1DCB25}" name="Table1" displayName="Table1" ref="A1:L176" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
   <autoFilter ref="A1:L176" xr:uid="{6C54116F-5E15-4235-9D70-EC1EDF1DCB25}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{308B0ED2-8B0D-41F9-8ACB-100444A53464}" name="RESMED SKU" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{3B825C44-7948-44AC-9BD6-668ED1180030}" name="RESMED DESCRIPTION" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{308B0ED2-8B0D-41F9-8ACB-100444A53464}" name=" SKU" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{3B825C44-7948-44AC-9BD6-668ED1180030}" name=" DESCRIPTION" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{B8D3D248-66E3-4DCD-B9AD-504D5F29767F}" name="Division Code" dataDxfId="9"/>
     <tableColumn id="4" xr3:uid="{8F723DC8-C966-4132-9DF2-FE22820AC0D1}" name="Product Group Code" dataDxfId="8"/>
     <tableColumn id="5" xr3:uid="{B49F0D17-2EB1-4BD3-97AF-22DFB97D2C9E}" name="Brand" dataDxfId="7"/>
@@ -2456,7 +2456,7 @@
     <tableColumn id="9" xr3:uid="{8411511A-394F-4CFF-990C-BC014F9EAAEE}" name="ITEM TRACKING CODE" dataDxfId="3"/>
     <tableColumn id="10" xr3:uid="{A54F2617-A9A6-4C73-9A5D-29909317B950}" name="GTIN.SKU" dataDxfId="2"/>
     <tableColumn id="11" xr3:uid="{3113F80C-A4A2-4BF5-99DD-3C2AD95072F2}" name="GTIN.Product Description" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{150BE031-6113-490C-9B37-0379A3CA89D6}" name="RESMED GTIN" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{150BE031-6113-490C-9B37-0379A3CA89D6}" name=" GTIN" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2761,13 +2761,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4140116-EBC3-4DB2-89A5-825E80AD1F2F}">
   <dimension ref="A1:L181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B181" sqref="B181"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.7265625" customWidth="1"/>
     <col min="2" max="2" width="52.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.453125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="20.453125" hidden="1" customWidth="1"/>
@@ -2783,10 +2783,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -2807,7 +2807,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>6</v>
@@ -2816,7 +2816,7 @@
         <v>7</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -9471,7 +9471,7 @@
     </row>
     <row r="181" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B181" s="3" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
     </row>
   </sheetData>
@@ -9483,6 +9483,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010074271C42279BD641A14F581AF600A089" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="02b9ae6d369ed40a39d9c470e85edae6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1d4d6a86-6f1e-4244-8667-b7d985b36c72" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e37bcbb0c76d164fb521241996f10478" ns2:_="">
     <xsd:import namespace="1d4d6a86-6f1e-4244-8667-b7d985b36c72"/>
@@ -9644,15 +9653,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -9660,6 +9660,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B88B85CB-18C6-4BF0-95FE-F88A6A026115}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED4FDCCB-8BF4-4384-BAF3-EE24D80335DE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9677,14 +9685,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B88B85CB-18C6-4BF0-95FE-F88A6A026115}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1178C89E-4DE0-43FB-84C6-FBB871E5EA3D}">
   <ds:schemaRefs>

</xml_diff>